<commit_message>
fix TAL production capacity issue and minor HP and TAL updates
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A_FGI_sugarcane.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A_FGI_sugarcane.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\repository_clones\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4459F49-05C7-4BA9-9F71-A79E502CEB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A3B659-6F7D-4EE4-B9D7-F805B2FBDCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -824,7 +824,7 @@
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD25"/>
+      <selection activeCell="E14" sqref="E14:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>